<commit_message>
Updated: marked materials that need to be moved and translated to md.
</commit_message>
<xml_diff>
--- a/TheoryAndExercisesToMD.xlsx
+++ b/TheoryAndExercisesToMD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h03181\Documents\Ohke\TheoryAndExercises to md\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h03180\työ\ohke\backend_3010\documentation-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4A973B4-D3DD-4A11-940F-7AD1D084AF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC4C74D-A78B-4D52-9AB1-E131000274B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11132BD7-7BD2-422D-A763-C88DFBF2EF22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="57">
   <si>
     <t>1hello_world</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Tehty/-</t>
   </si>
   <si>
-    <t>Toiminto: siirto/poisto</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -198,6 +195,18 @@
   </si>
   <si>
     <t>Siniset alasvetolaatikot: mitä tehdään tiedoston kanssa ja onko tehty vai ei</t>
+  </si>
+  <si>
+    <t>siirto</t>
+  </si>
+  <si>
+    <t>Toiminto: siirto/ei siirto</t>
+  </si>
+  <si>
+    <t>ei md:ksi</t>
+  </si>
+  <si>
+    <t>sensuroi</t>
   </si>
 </sst>
 </file>
@@ -250,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -532,11 +541,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -567,7 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -616,6 +665,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -625,8 +683,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,11 +1032,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C414C6-FBA4-4C97-AEC3-D7EBC9B0724A}">
-  <dimension ref="D1:L44"/>
+  <dimension ref="D1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,11 +1047,12 @@
     <col min="6" max="6" width="5.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:12" s="19" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="4:13" s="19" customFormat="1" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D1" s="18"/>
       <c r="F1" s="20" t="s">
         <v>9</v>
@@ -992,31 +1063,33 @@
       <c r="H1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="I1" s="20"/>
       <c r="J1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D2" s="29" t="s">
+    </row>
+    <row r="2" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="21"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="30"/>
       <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D3" s="9"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
@@ -1028,14 +1101,15 @@
         <v>12</v>
       </c>
       <c r="H3" s="14"/>
-      <c r="I3" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I3" s="35"/>
       <c r="J3" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D4" s="9"/>
       <c r="E4" s="4" t="s">
         <v>2</v>
@@ -1047,14 +1121,15 @@
       <c r="H4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I4" s="35"/>
       <c r="J4" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
         <v>3</v>
@@ -1066,14 +1141,15 @@
       <c r="H5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I5" s="35"/>
       <c r="J5" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D6" s="9"/>
       <c r="E6" s="4" t="s">
         <v>4</v>
@@ -1083,14 +1159,15 @@
       <c r="H6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I6" s="35"/>
       <c r="J6" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D7" s="9"/>
       <c r="E7" s="4" t="s">
         <v>5</v>
@@ -1102,14 +1179,15 @@
       <c r="H7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I7" s="35"/>
       <c r="J7" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D8" s="9"/>
       <c r="E8" s="4" t="s">
         <v>6</v>
@@ -1121,14 +1199,15 @@
         <v>12</v>
       </c>
       <c r="H8" s="14"/>
-      <c r="I8" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I8" s="35"/>
       <c r="J8" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D9" s="9"/>
       <c r="E9" s="4" t="s">
         <v>7</v>
@@ -1140,14 +1219,15 @@
         <v>12</v>
       </c>
       <c r="H9" s="14"/>
-      <c r="I9" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I9" s="35"/>
       <c r="J9" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="10"/>
       <c r="E10" s="7" t="s">
         <v>8</v>
@@ -1159,25 +1239,27 @@
         <v>12</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D11" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="21"/>
-    </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D12" s="9"/>
       <c r="E12" s="4" t="s">
         <v>14</v>
@@ -1189,14 +1271,15 @@
       <c r="H12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="I12" s="35"/>
+      <c r="J12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D13" s="9"/>
       <c r="E13" s="4" t="s">
         <v>15</v>
@@ -1208,14 +1291,15 @@
       <c r="H13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="I13" s="35"/>
+      <c r="J13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" s="4" t="s">
         <v>16</v>
@@ -1227,14 +1311,15 @@
       <c r="H14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="I14" s="35"/>
+      <c r="J14" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D15" s="9"/>
       <c r="E15" s="4" t="s">
         <v>17</v>
@@ -1244,14 +1329,15 @@
         <v>12</v>
       </c>
       <c r="H15" s="14"/>
-      <c r="I15" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="I15" s="35"/>
+      <c r="J15" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D16" s="9"/>
       <c r="E16" s="4" t="s">
         <v>18</v>
@@ -1261,14 +1347,15 @@
       <c r="H16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I16" s="35"/>
+      <c r="J16" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" s="4" t="s">
         <v>19</v>
@@ -1278,14 +1365,15 @@
         <v>12</v>
       </c>
       <c r="H17" s="14"/>
-      <c r="I17" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I17" s="35"/>
+      <c r="J17" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" s="4" t="s">
         <v>20</v>
@@ -1295,14 +1383,15 @@
       <c r="H18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I18" s="35"/>
+      <c r="J18" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" s="4" t="s">
         <v>21</v>
@@ -1314,14 +1403,15 @@
       <c r="H19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="35"/>
+      <c r="J19" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="11"/>
       <c r="E20" s="13" t="s">
         <v>22</v>
@@ -1333,25 +1423,27 @@
         <v>12</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D21" s="29" t="s">
+      <c r="I20" s="37"/>
+      <c r="J20" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D21" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="21"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="30"/>
       <c r="J21" s="21"/>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="21"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D22" s="9"/>
       <c r="E22" s="4" t="s">
         <v>24</v>
@@ -1361,14 +1453,15 @@
         <v>12</v>
       </c>
       <c r="H22" s="14"/>
-      <c r="I22" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I22" s="35"/>
       <c r="J22" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D23" s="9"/>
       <c r="E23" s="4" t="s">
         <v>25</v>
@@ -1380,14 +1473,15 @@
       <c r="H23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I23" s="35"/>
       <c r="J23" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="E24" s="4" t="s">
         <v>26</v>
@@ -1399,14 +1493,15 @@
       <c r="H24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I24" s="35"/>
       <c r="J24" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="E25" s="4" t="s">
         <v>27</v>
@@ -1418,14 +1513,15 @@
         <v>12</v>
       </c>
       <c r="H25" s="14"/>
-      <c r="I25" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I25" s="35"/>
       <c r="J25" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="E26" s="4" t="s">
         <v>28</v>
@@ -1437,14 +1533,15 @@
         <v>12</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I26" s="35"/>
       <c r="J26" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D27" s="11"/>
       <c r="E27" s="13" t="s">
         <v>29</v>
@@ -1454,25 +1551,27 @@
         <v>12</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="I27" s="38"/>
       <c r="J27" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D28" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D28" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="25"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="39"/>
       <c r="J28" s="25"/>
-    </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="25"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D29" s="9"/>
       <c r="E29" s="4" t="s">
         <v>31</v>
@@ -1484,14 +1583,15 @@
       <c r="H29" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I29" s="35"/>
       <c r="J29" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D30" s="9"/>
       <c r="E30" s="4" t="s">
         <v>32</v>
@@ -1501,14 +1601,15 @@
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="14"/>
-      <c r="I30" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I30" s="35"/>
       <c r="J30" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D31" s="11"/>
       <c r="E31" s="13" t="s">
         <v>33</v>
@@ -1520,25 +1621,27 @@
         <v>12</v>
       </c>
       <c r="H31" s="15"/>
-      <c r="I31" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="J31" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D32" s="29" t="s">
+      <c r="I31" s="37"/>
+      <c r="J31" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D32" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="21"/>
-    </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="21"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
       <c r="E33" s="4" t="s">
         <v>35</v>
@@ -1550,14 +1653,17 @@
         <v>12</v>
       </c>
       <c r="H33" s="14"/>
-      <c r="I33" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I33" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="E34" s="4" t="s">
         <v>36</v>
@@ -1569,14 +1675,15 @@
       <c r="H34" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I34" s="35"/>
+      <c r="J34" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="E35" s="4" t="s">
         <v>37</v>
@@ -1588,14 +1695,15 @@
         <v>12</v>
       </c>
       <c r="H35" s="14"/>
-      <c r="I35" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I35" s="35"/>
+      <c r="J35" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="E36" s="4" t="s">
         <v>38</v>
@@ -1607,14 +1715,15 @@
         <v>12</v>
       </c>
       <c r="H36" s="14"/>
-      <c r="I36" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I36" s="35"/>
+      <c r="J36" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="E37" s="4" t="s">
         <v>39</v>
@@ -1624,14 +1733,15 @@
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="14"/>
-      <c r="I37" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="35"/>
+      <c r="J37" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1645,14 +1755,15 @@
         <v>12</v>
       </c>
       <c r="H38" s="14"/>
-      <c r="I38" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I38" s="35"/>
+      <c r="J38" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="11"/>
       <c r="E39" s="13" t="s">
         <v>42</v>
@@ -1664,25 +1775,27 @@
         <v>12</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="I39" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D40" s="29" t="s">
+      <c r="I39" s="38"/>
+      <c r="J39" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D40" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="21"/>
-    </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="21"/>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="E41" s="4" t="s">
         <v>44</v>
@@ -1694,14 +1807,17 @@
       <c r="H41" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="16" t="s">
-        <v>51</v>
+      <c r="I41" s="35" t="s">
+        <v>56</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="E42" s="4" t="s">
         <v>45</v>
@@ -1713,14 +1829,15 @@
         <v>12</v>
       </c>
       <c r="H42" s="14"/>
-      <c r="I42" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I42" s="35"/>
       <c r="J42" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D43" s="9"/>
       <c r="E43" s="4" t="s">
         <v>46</v>
@@ -1732,14 +1849,15 @@
       <c r="H43" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I43" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="I43" s="35"/>
       <c r="J43" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D44" s="11"/>
       <c r="E44" s="13" t="s">
         <v>47</v>
@@ -1751,27 +1869,28 @@
         <v>12</v>
       </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="I44" s="38"/>
       <c r="J44" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K44" s="17" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D2:H2"/>
     <mergeCell ref="D40:H40"/>
     <mergeCell ref="D32:H32"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D2:H2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J22:J27 J3:J10 J12:J20 J29:J31 J33:J39 J41:J44" xr:uid="{F1D58062-0363-4E68-A2D2-85319596AFB3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K22:K27 K3:K10 K12:K20 K29:K31 K33:K39 K41:K44" xr:uid="{F1D58062-0363-4E68-A2D2-85319596AFB3}">
       <formula1>"tehty,-"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I44" xr:uid="{76217A6F-5A28-40CF-8D98-41FDF7042767}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J44" xr:uid="{76217A6F-5A28-40CF-8D98-41FDF7042767}">
       <formula1>"?,siirto,poisto"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changed: 'poista' -> 'ei siirto', ICE added screeshot
</commit_message>
<xml_diff>
--- a/TheoryAndExercisesToMD.xlsx
+++ b/TheoryAndExercisesToMD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h03180\työ\ohke\backend_3010\documentation-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia-my.sharepoint.com/personal/h03181_haaga-helia_fi/Documents/Documents/HH documentation Github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC4C74D-A78B-4D52-9AB1-E131000274B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{CFC4C74D-A78B-4D52-9AB1-E131000274B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{688CB853-F33E-45C9-A36E-FBD8AECB8799}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11132BD7-7BD2-422D-A763-C88DFBF2EF22}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{11132BD7-7BD2-422D-A763-C88DFBF2EF22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="58">
   <si>
     <t>1hello_world</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Tehty/-</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>&lt;--</t>
   </si>
   <si>
@@ -207,6 +204,12 @@
   </si>
   <si>
     <t>sensuroi</t>
+  </si>
+  <si>
+    <t>Kuvakaappaus versiosta 4.3.2025:</t>
+  </si>
+  <si>
+    <t>ei siirto</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -461,33 +464,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -509,34 +486,10 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -585,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -644,26 +597,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -671,33 +639,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,6 +655,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>16801</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>54187</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47FDE193-25F6-4909-B9AB-9FE8728F6CBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11668125" y="1609725"/>
+          <a:ext cx="6107086" cy="6555952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1032,11 +1023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C414C6-FBA4-4C97-AEC3-D7EBC9B0724A}">
-  <dimension ref="D1:M44"/>
+  <dimension ref="D1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,7 +1043,7 @@
     <col min="11" max="11" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:13" s="19" customFormat="1" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="4:16" s="19" customFormat="1" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D1" s="18"/>
       <c r="F1" s="20" t="s">
         <v>9</v>
@@ -1065,31 +1056,31 @@
       </c>
       <c r="I1" s="20"/>
       <c r="J1" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D2" s="32" t="s">
+    </row>
+    <row r="2" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="30"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="26"/>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
     </row>
-    <row r="3" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D3" s="9"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
@@ -1101,15 +1092,15 @@
         <v>12</v>
       </c>
       <c r="H3" s="14"/>
-      <c r="I3" s="35"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="16" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D4" s="9"/>
       <c r="E4" s="4" t="s">
         <v>2</v>
@@ -1121,15 +1112,15 @@
       <c r="H4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
         <v>3</v>
@@ -1141,15 +1132,15 @@
       <c r="H5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="16" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D6" s="9"/>
       <c r="E6" s="4" t="s">
         <v>4</v>
@@ -1159,15 +1150,18 @@
       <c r="H6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="16" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="P6" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D7" s="9"/>
       <c r="E7" s="4" t="s">
         <v>5</v>
@@ -1179,15 +1173,15 @@
       <c r="H7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="35"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D8" s="9"/>
       <c r="E8" s="4" t="s">
         <v>6</v>
@@ -1199,15 +1193,15 @@
         <v>12</v>
       </c>
       <c r="H8" s="14"/>
-      <c r="I8" s="35"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D9" s="9"/>
       <c r="E9" s="4" t="s">
         <v>7</v>
@@ -1219,15 +1213,15 @@
         <v>12</v>
       </c>
       <c r="H9" s="14"/>
-      <c r="I9" s="35"/>
+      <c r="I9" s="28"/>
       <c r="J9" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="4:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="10"/>
       <c r="E10" s="7" t="s">
         <v>8</v>
@@ -1240,26 +1234,26 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="17" t="s">
-        <v>53</v>
+      <c r="J10" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D11" s="32" t="s">
+    <row r="11" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D11" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="29"/>
       <c r="J11" s="22"/>
       <c r="K11" s="21"/>
     </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D12" s="9"/>
       <c r="E12" s="4" t="s">
         <v>14</v>
@@ -1271,15 +1265,15 @@
       <c r="H12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="35"/>
-      <c r="J12" s="23" t="s">
-        <v>53</v>
+      <c r="I12" s="28"/>
+      <c r="J12" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D13" s="9"/>
       <c r="E13" s="4" t="s">
         <v>15</v>
@@ -1291,15 +1285,15 @@
       <c r="H13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="35"/>
-      <c r="J13" s="23" t="s">
-        <v>50</v>
+      <c r="I13" s="28"/>
+      <c r="J13" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" s="4" t="s">
         <v>16</v>
@@ -1311,15 +1305,15 @@
       <c r="H14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="35"/>
-      <c r="J14" s="23" t="s">
-        <v>53</v>
+      <c r="I14" s="28"/>
+      <c r="J14" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D15" s="9"/>
       <c r="E15" s="4" t="s">
         <v>17</v>
@@ -1329,15 +1323,15 @@
         <v>12</v>
       </c>
       <c r="H15" s="14"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="23" t="s">
-        <v>53</v>
+      <c r="I15" s="28"/>
+      <c r="J15" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D16" s="9"/>
       <c r="E16" s="4" t="s">
         <v>18</v>
@@ -1347,9 +1341,9 @@
       <c r="H16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="23" t="s">
-        <v>53</v>
+      <c r="I16" s="28"/>
+      <c r="J16" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>48</v>
@@ -1365,9 +1359,9 @@
         <v>12</v>
       </c>
       <c r="H17" s="14"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="23" t="s">
-        <v>53</v>
+      <c r="I17" s="28"/>
+      <c r="J17" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K17" s="16" t="s">
         <v>48</v>
@@ -1383,9 +1377,9 @@
       <c r="H18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="35"/>
-      <c r="J18" s="23" t="s">
-        <v>53</v>
+      <c r="I18" s="28"/>
+      <c r="J18" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>48</v>
@@ -1403,9 +1397,9 @@
       <c r="H19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="23" t="s">
-        <v>53</v>
+      <c r="I19" s="28"/>
+      <c r="J19" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>48</v>
@@ -1423,23 +1417,23 @@
         <v>12</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="24" t="s">
-        <v>53</v>
+      <c r="I20" s="30"/>
+      <c r="J20" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="30"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="26"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
     </row>
@@ -1453,9 +1447,9 @@
         <v>12</v>
       </c>
       <c r="H22" s="14"/>
-      <c r="I22" s="35"/>
+      <c r="I22" s="28"/>
       <c r="J22" s="16" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>48</v>
@@ -1473,9 +1467,9 @@
       <c r="H23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="35"/>
+      <c r="I23" s="28"/>
       <c r="J23" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>48</v>
@@ -1493,9 +1487,9 @@
       <c r="H24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="35"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>48</v>
@@ -1513,9 +1507,9 @@
         <v>12</v>
       </c>
       <c r="H25" s="14"/>
-      <c r="I25" s="35"/>
+      <c r="I25" s="28"/>
       <c r="J25" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>48</v>
@@ -1533,9 +1527,9 @@
         <v>12</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="35"/>
+      <c r="I26" s="28"/>
       <c r="J26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>48</v>
@@ -1551,25 +1545,25 @@
         <v>12</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="17" t="s">
-        <v>50</v>
+      <c r="I27" s="31"/>
+      <c r="J27" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K27" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D29" s="9"/>
@@ -1583,9 +1577,9 @@
       <c r="H29" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="35"/>
+      <c r="I29" s="28"/>
       <c r="J29" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K29" s="16" t="s">
         <v>48</v>
@@ -1601,9 +1595,9 @@
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="14"/>
-      <c r="I30" s="35"/>
+      <c r="I30" s="28"/>
       <c r="J30" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K30" s="16" t="s">
         <v>48</v>
@@ -1621,24 +1615,24 @@
         <v>12</v>
       </c>
       <c r="H31" s="15"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="26" t="s">
-        <v>53</v>
+      <c r="I31" s="30"/>
+      <c r="J31" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K31" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="27"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="24"/>
       <c r="K32" s="21"/>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.3">
@@ -1653,11 +1647,11 @@
         <v>12</v>
       </c>
       <c r="H33" s="14"/>
-      <c r="I33" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="J33" s="23" t="s">
-        <v>53</v>
+      <c r="I33" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K33" s="16" t="s">
         <v>48</v>
@@ -1675,9 +1669,9 @@
       <c r="H34" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="35"/>
-      <c r="J34" s="23" t="s">
-        <v>53</v>
+      <c r="I34" s="28"/>
+      <c r="J34" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K34" s="16" t="s">
         <v>48</v>
@@ -1695,9 +1689,9 @@
         <v>12</v>
       </c>
       <c r="H35" s="14"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="23" t="s">
-        <v>53</v>
+      <c r="I35" s="28"/>
+      <c r="J35" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K35" s="16" t="s">
         <v>48</v>
@@ -1715,9 +1709,9 @@
         <v>12</v>
       </c>
       <c r="H36" s="14"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="23" t="s">
-        <v>53</v>
+      <c r="I36" s="28"/>
+      <c r="J36" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K36" s="16" t="s">
         <v>48</v>
@@ -1733,9 +1727,9 @@
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="14"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="23" t="s">
-        <v>50</v>
+      <c r="I37" s="28"/>
+      <c r="J37" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K37" s="16" t="s">
         <v>48</v>
@@ -1755,9 +1749,9 @@
         <v>12</v>
       </c>
       <c r="H38" s="14"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="23" t="s">
-        <v>50</v>
+      <c r="I38" s="28"/>
+      <c r="J38" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K38" s="16" t="s">
         <v>48</v>
@@ -1775,24 +1769,24 @@
         <v>12</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="28" t="s">
-        <v>50</v>
+      <c r="I39" s="31"/>
+      <c r="J39" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K39" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D40" s="32" t="s">
+      <c r="D40" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="25"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="23"/>
       <c r="K40" s="21"/>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.3">
@@ -1807,11 +1801,11 @@
       <c r="H41" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="35" t="s">
-        <v>56</v>
+      <c r="I41" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K41" s="16" t="s">
         <v>48</v>
@@ -1829,9 +1823,9 @@
         <v>12</v>
       </c>
       <c r="H42" s="14"/>
-      <c r="I42" s="35"/>
+      <c r="I42" s="28"/>
       <c r="J42" s="16" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K42" s="16" t="s">
         <v>48</v>
@@ -1849,9 +1843,9 @@
       <c r="H43" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I43" s="35"/>
+      <c r="I43" s="28"/>
       <c r="J43" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K43" s="16" t="s">
         <v>48</v>
@@ -1869,9 +1863,9 @@
         <v>12</v>
       </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="17" t="s">
-        <v>53</v>
+      <c r="I44" s="31"/>
+      <c r="J44" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="K44" s="17" t="s">
         <v>48</v>
@@ -1886,14 +1880,18 @@
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D11:H11"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K22:K27 K3:K10 K12:K20 K29:K31 K33:K39 K41:K44" xr:uid="{F1D58062-0363-4E68-A2D2-85319596AFB3}">
       <formula1>"tehty,-"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J44" xr:uid="{76217A6F-5A28-40CF-8D98-41FDF7042767}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 J11 J21 J28 J32 J40" xr:uid="{8403F6B4-ABCC-4817-B246-3C01BB7A8337}">
       <formula1>"?,siirto,poisto"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J10 J12:J20 J22:J27 J29:J31 J33:J39 J41:J44" xr:uid="{18849C46-C436-430C-8567-17BB7222A414}">
+      <formula1>"?,siirto,ei siirto"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>